<commit_message>
Figure 9 bin code updated
</commit_message>
<xml_diff>
--- a/BarGraphIntValues.xlsx
+++ b/BarGraphIntValues.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="33960" windowHeight="22920" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Picopro" sheetId="1" r:id="rId1"/>
     <sheet name="PicoEuk" sheetId="2" r:id="rId2"/>
     <sheet name="Nanoeuk" sheetId="3" r:id="rId3"/>
+    <sheet name="Prochlorococcus" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="13">
   <si>
     <t>SSTFZ</t>
   </si>
@@ -42,6 +43,24 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>pro</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>prym</t>
+  </si>
+  <si>
+    <t>pel</t>
+  </si>
+  <si>
+    <t>diat</t>
+  </si>
+  <si>
+    <t>dino</t>
   </si>
 </sst>
 </file>
@@ -90,8 +109,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -124,7 +155,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -139,6 +170,12 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -153,6 +190,12 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -673,7 +716,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -814,4 +857,393 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>2008</v>
+      </c>
+      <c r="B2">
+        <v>10.669241169768499</v>
+      </c>
+      <c r="C2">
+        <v>11.036368433795699</v>
+      </c>
+      <c r="D2">
+        <v>12.574399891002001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2009</v>
+      </c>
+      <c r="B3">
+        <v>9.29659788845278</v>
+      </c>
+      <c r="C3">
+        <v>9.2721718993483595</v>
+      </c>
+      <c r="D3">
+        <v>7.85022260201852</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>2011</v>
+      </c>
+      <c r="B4">
+        <v>8.4338064603843801</v>
+      </c>
+      <c r="C4">
+        <v>9.99501439400699</v>
+      </c>
+      <c r="D4">
+        <v>5.0995914842007597</v>
+      </c>
+      <c r="G4">
+        <v>2008</v>
+      </c>
+      <c r="H4">
+        <v>2009</v>
+      </c>
+      <c r="I4">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>10.669241169768499</v>
+      </c>
+      <c r="H5">
+        <v>9.29659788845278</v>
+      </c>
+      <c r="I5">
+        <v>8.4338064603843801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>11.036368433795699</v>
+      </c>
+      <c r="H6">
+        <v>9.2721718993483595</v>
+      </c>
+      <c r="I6">
+        <v>9.99501439400699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>12.574399891002001</v>
+      </c>
+      <c r="H7">
+        <v>7.85022260201852</v>
+      </c>
+      <c r="I7">
+        <v>5.0995914842007597</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1.1999081119239501</v>
+      </c>
+      <c r="H8">
+        <v>1.69803858625285</v>
+      </c>
+      <c r="I8">
+        <v>2.4738192058861301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>9.3806301862975907</v>
+      </c>
+      <c r="H9">
+        <v>6.4848959764837399</v>
+      </c>
+      <c r="I9">
+        <v>7.2175811584779801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>5.2061973246467499</v>
+      </c>
+      <c r="H10">
+        <v>6.3787859028797298</v>
+      </c>
+      <c r="I10">
+        <v>7.0733332657798602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>4.3791405733248503</v>
+      </c>
+      <c r="H11">
+        <v>5.1112931369220096</v>
+      </c>
+      <c r="I11">
+        <v>20.9120246379109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>5.6785397552696697</v>
+      </c>
+      <c r="H12">
+        <v>5.5545428245241499</v>
+      </c>
+      <c r="I12">
+        <v>10.2989110906904</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>5.9980387631758401</v>
+      </c>
+      <c r="H13">
+        <v>7.8744218804181596</v>
+      </c>
+      <c r="I13">
+        <v>12.2534389906515</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1.5175168297952599</v>
+      </c>
+      <c r="H14">
+        <v>2.4985135210647802</v>
+      </c>
+      <c r="I14">
+        <v>7.8868582706322004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>2.1770540783253698</v>
+      </c>
+      <c r="H15">
+        <v>1.79932772327945</v>
+      </c>
+      <c r="I15">
+        <v>3.04275348137153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3.1377489187943799</v>
+      </c>
+      <c r="H16">
+        <v>3.96425629646096</v>
+      </c>
+      <c r="I16">
+        <v>6.5479707580796402</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9">
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0.173197233838458</v>
+      </c>
+      <c r="H17">
+        <v>0.155046582277342</v>
+      </c>
+      <c r="I17">
+        <v>0.57203962039999301</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9">
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0.50758451990865505</v>
+      </c>
+      <c r="H18">
+        <v>0.31582691707104898</v>
+      </c>
+      <c r="I18">
+        <v>0.64852488447193601</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9">
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>0.29172129452894502</v>
+      </c>
+      <c r="H19">
+        <v>0.359610481236946</v>
+      </c>
+      <c r="I19">
+        <v>1.1524068770184299</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9">
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0.10006324546170201</v>
+      </c>
+      <c r="H20">
+        <v>6.2378783538737999E-2</v>
+      </c>
+      <c r="I20">
+        <v>0.72303276701368102</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9">
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>9.3593347037130403E-2</v>
+      </c>
+      <c r="I21">
+        <v>0.27352451322719501</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9">
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>0.30915258179740701</v>
+      </c>
+      <c r="H22">
+        <v>0.339995767151825</v>
+      </c>
+      <c r="I22">
+        <v>0.50690302800549603</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>